<commit_message>
Elec sector calibration edits
</commit_message>
<xml_diff>
--- a/InputData/elec/BHRbEF/BAU Heat Rate by Electricity Fuel.xlsx
+++ b/InputData/elec/BHRbEF/BAU Heat Rate by Electricity Fuel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iamho\Dropbox\Energy Innovation\InputData_RevisionComplete\elec\BHRbEF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-southkorea\InputData\elec\BHRbEF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE76AE3-618B-48E2-89CC-54BDA049BEFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973C5770-C914-4F63-970F-96E30DA96C55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9240" yWindow="1190" windowWidth="28090" windowHeight="18220" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,8 @@
     <sheet name="heat of nuclear gen" sheetId="21" r:id="rId4"/>
     <sheet name="outlook of power" sheetId="20" r:id="rId5"/>
     <sheet name="Cal" sheetId="14" r:id="rId6"/>
-    <sheet name="BHRbEF" sheetId="17" r:id="rId7"/>
+    <sheet name="US values" sheetId="22" r:id="rId7"/>
+    <sheet name="BHRbEF" sheetId="17" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="212">
   <si>
     <t>BAU Heat Rate by Electricity Fuel</t>
   </si>
@@ -142,7 +143,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -153,7 +154,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1018,21 +1019,24 @@
     <t>Power generation by scenario</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
+  <si>
+    <t>Where there is no Korea data available, we use US values from the US EPS.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="0.0%"/>
-    <numFmt numFmtId="177" formatCode="#,##0.0#"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0#"/>
   </numFmts>
   <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1040,7 +1044,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1048,7 +1052,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1060,7 +1064,7 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1068,7 +1072,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1082,7 +1086,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1131,7 +1135,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1161,7 +1165,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1169,7 +1173,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1177,7 +1181,7 @@
     <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -1457,7 +1461,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
@@ -1556,10 +1560,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1589,27 +1593,27 @@
     <xf numFmtId="4" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="15" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="16" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="20" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1619,7 +1623,7 @@
     <xf numFmtId="0" fontId="21" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1648,10 +1652,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1660,22 +1673,13 @@
     <xf numFmtId="0" fontId="13" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="5">
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="메모" xfId="4" builtinId="10"/>
-    <cellStyle name="쉼표 [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
-    <cellStyle name="하이퍼링크" xfId="1" builtinId="8"/>
+    <cellStyle name="Note" xfId="4" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2002,18 +2006,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V40"/>
+  <dimension ref="A1:V42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9" style="4"/>
-    <col min="2" max="2" width="63.75" style="4" customWidth="1"/>
+    <col min="2" max="2" width="63.7109375" style="4" customWidth="1"/>
     <col min="3" max="3" width="9" style="4"/>
-    <col min="4" max="4" width="9.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
@@ -2376,6 +2380,11 @@
     <row r="40" spans="1:22">
       <c r="A40" s="4" t="s">
         <v>200</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22">
+      <c r="A42" s="4" t="s">
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -2400,9 +2409,9 @@
       <selection activeCell="E104" sqref="E104"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="9" width="23.5" style="4" customWidth="1"/>
+    <col min="1" max="9" width="23.42578125" style="4" customWidth="1"/>
     <col min="10" max="16384" width="8" style="4"/>
   </cols>
   <sheetData>
@@ -5152,7 +5161,7 @@
         <v>-7</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="17.5" thickBot="1"/>
+    <row r="100" spans="1:9" ht="15.75" thickBot="1"/>
     <row r="101" spans="1:9">
       <c r="A101" s="5"/>
       <c r="B101" s="6">
@@ -5189,7 +5198,7 @@
         <v>285173</v>
       </c>
     </row>
-    <row r="103" spans="1:9">
+    <row r="103" spans="1:9" ht="16.5">
       <c r="A103" s="12" t="s">
         <v>33</v>
       </c>
@@ -5249,7 +5258,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="106" spans="1:9">
+    <row r="106" spans="1:9" ht="16.5">
       <c r="A106" s="12" t="s">
         <v>37</v>
       </c>
@@ -5263,7 +5272,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="107" spans="1:9" ht="17.5" thickBot="1">
+    <row r="107" spans="1:9" ht="15.75" thickBot="1">
       <c r="A107" s="17"/>
       <c r="B107" s="18"/>
       <c r="C107" s="18"/>
@@ -5288,12 +5297,12 @@
         <v>93</v>
       </c>
     </row>
-    <row r="110" spans="1:9">
+    <row r="110" spans="1:9" ht="16.5">
       <c r="A110" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="111" spans="1:9">
+    <row r="111" spans="1:9" ht="16.5">
       <c r="A111" s="26"/>
       <c r="D111" s="27" t="s">
         <v>95</v>
@@ -5328,25 +5337,25 @@
       <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.08203125" style="43" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.58203125" style="43" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" style="43" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.58203125" style="43" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.58203125" style="43" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.58203125" style="43" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.58203125" style="43" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.58203125" style="43" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.58203125" style="43" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="12.58203125" style="43" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="11.58203125" style="43" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.33203125" style="43" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="12.58203125" style="43" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.58203125" style="43" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="11.58203125" style="43" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="12.58203125" style="43" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="11.5" style="43" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="43" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.5703125" style="43" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" style="43" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.5703125" style="43" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" style="43" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" style="43" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" style="43" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.5703125" style="43" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" style="43" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="12.5703125" style="43" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="11.5703125" style="43" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.28515625" style="43" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="12.5703125" style="43" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.5703125" style="43" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="11.5703125" style="43" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="12.5703125" style="43" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="11.42578125" style="43" bestFit="1" customWidth="1"/>
     <col min="27" max="16384" width="9" style="43"/>
   </cols>
   <sheetData>
@@ -5356,35 +5365,35 @@
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="73" t="s">
+      <c r="A2" s="69" t="s">
         <v>108</v>
       </c>
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="69" t="s">
         <v>109</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73" t="s">
+      <c r="C2" s="69"/>
+      <c r="D2" s="69" t="s">
         <v>110</v>
       </c>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73" t="s">
+      <c r="E2" s="69"/>
+      <c r="F2" s="69" t="s">
         <v>111</v>
       </c>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73" t="s">
+      <c r="G2" s="69"/>
+      <c r="H2" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="73"/>
-      <c r="J2" s="73" t="s">
+      <c r="I2" s="69"/>
+      <c r="J2" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="K2" s="73"/>
-      <c r="L2" s="73" t="s">
+      <c r="K2" s="69"/>
+      <c r="L2" s="69" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="17.5" thickBot="1">
-      <c r="A3" s="74"/>
+    <row r="3" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A3" s="70"/>
       <c r="B3" s="37" t="s">
         <v>113</v>
       </c>
@@ -5415,9 +5424,9 @@
       <c r="K3" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="L3" s="74"/>
-    </row>
-    <row r="4" spans="1:12" ht="17.5" thickTop="1">
+      <c r="L3" s="70"/>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" thickTop="1">
       <c r="A4" s="44">
         <v>2020</v>
       </c>
@@ -5844,37 +5853,37 @@
       </c>
     </row>
     <row r="17" spans="1:26">
-      <c r="A17" s="70" t="s">
+      <c r="A17" s="71" t="s">
         <v>108</v>
       </c>
-      <c r="B17" s="73" t="s">
+      <c r="B17" s="69" t="s">
         <v>132</v>
       </c>
-      <c r="C17" s="73"/>
-      <c r="D17" s="73"/>
-      <c r="E17" s="70"/>
-      <c r="F17" s="69" t="s">
+      <c r="C17" s="69"/>
+      <c r="D17" s="69"/>
+      <c r="E17" s="71"/>
+      <c r="F17" s="73" t="s">
         <v>116</v>
       </c>
-      <c r="G17" s="73"/>
-      <c r="H17" s="73"/>
-      <c r="I17" s="73"/>
-      <c r="J17" s="70"/>
-      <c r="K17" s="69" t="s">
+      <c r="G17" s="69"/>
+      <c r="H17" s="69"/>
+      <c r="I17" s="69"/>
+      <c r="J17" s="71"/>
+      <c r="K17" s="73" t="s">
         <v>134</v>
       </c>
-      <c r="L17" s="73"/>
-      <c r="M17" s="70"/>
-      <c r="N17" s="71" t="s">
+      <c r="L17" s="69"/>
+      <c r="M17" s="71"/>
+      <c r="N17" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="O17" s="71" t="s">
+      <c r="O17" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="P17" s="71" t="s">
+      <c r="P17" s="74" t="s">
         <v>117</v>
       </c>
-      <c r="Q17" s="71" t="s">
+      <c r="Q17" s="74" t="s">
         <v>118</v>
       </c>
       <c r="R17" s="41" t="s">
@@ -5883,24 +5892,24 @@
       <c r="S17" s="41" t="s">
         <v>136</v>
       </c>
-      <c r="T17" s="71" t="s">
+      <c r="T17" s="74" t="s">
         <v>29</v>
       </c>
-      <c r="U17" s="71" t="s">
+      <c r="U17" s="74" t="s">
         <v>52</v>
       </c>
-      <c r="V17" s="69" t="s">
+      <c r="V17" s="73" t="s">
         <v>119</v>
       </c>
-      <c r="W17" s="73"/>
-      <c r="X17" s="70"/>
-      <c r="Y17" s="69" t="s">
+      <c r="W17" s="69"/>
+      <c r="X17" s="71"/>
+      <c r="Y17" s="73" t="s">
         <v>120</v>
       </c>
-      <c r="Z17" s="70"/>
-    </row>
-    <row r="18" spans="1:26" ht="32.5" thickBot="1">
-      <c r="A18" s="75"/>
+      <c r="Z17" s="71"/>
+    </row>
+    <row r="18" spans="1:26" ht="27.75" thickBot="1">
+      <c r="A18" s="72"/>
       <c r="B18" s="37" t="s">
         <v>121</v>
       </c>
@@ -5937,18 +5946,18 @@
       <c r="M18" s="38" t="s">
         <v>125</v>
       </c>
-      <c r="N18" s="72"/>
-      <c r="O18" s="72"/>
-      <c r="P18" s="72"/>
-      <c r="Q18" s="72"/>
+      <c r="N18" s="75"/>
+      <c r="O18" s="75"/>
+      <c r="P18" s="75"/>
+      <c r="Q18" s="75"/>
       <c r="R18" s="40" t="s">
         <v>137</v>
       </c>
       <c r="S18" s="40" t="s">
         <v>137</v>
       </c>
-      <c r="T18" s="72"/>
-      <c r="U18" s="72"/>
+      <c r="T18" s="75"/>
+      <c r="U18" s="75"/>
       <c r="V18" s="39" t="s">
         <v>126</v>
       </c>
@@ -5965,7 +5974,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="19" spans="1:26" ht="17.5" thickTop="1">
+    <row r="19" spans="1:26" ht="15.75" thickTop="1">
       <c r="A19" s="44">
         <v>2020</v>
       </c>
@@ -6872,6 +6881,14 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="Y17:Z17"/>
+    <mergeCell ref="N17:N18"/>
+    <mergeCell ref="O17:O18"/>
+    <mergeCell ref="P17:P18"/>
+    <mergeCell ref="Q17:Q18"/>
+    <mergeCell ref="T17:T18"/>
+    <mergeCell ref="U17:U18"/>
+    <mergeCell ref="V17:X17"/>
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="B17:E17"/>
@@ -6883,14 +6900,6 @@
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="J2:K2"/>
-    <mergeCell ref="Y17:Z17"/>
-    <mergeCell ref="N17:N18"/>
-    <mergeCell ref="O17:O18"/>
-    <mergeCell ref="P17:P18"/>
-    <mergeCell ref="Q17:Q18"/>
-    <mergeCell ref="T17:T18"/>
-    <mergeCell ref="U17:U18"/>
-    <mergeCell ref="V17:X17"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6905,9 +6914,9 @@
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="1:12" s="52" customFormat="1" ht="26.15" customHeight="1">
+    <row r="2" spans="1:12" s="52" customFormat="1" ht="26.1" customHeight="1">
       <c r="A2" s="56" t="s">
         <v>164</v>
       </c>
@@ -7871,7 +7880,7 @@
       <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="9" customWidth="1"/>
   </cols>
@@ -8102,14 +8111,14 @@
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.5" style="28" customWidth="1"/>
-    <col min="2" max="2" width="32.75" style="28" customWidth="1"/>
-    <col min="3" max="3" width="19.58203125" style="28" customWidth="1"/>
-    <col min="4" max="4" width="27.75" style="28" customWidth="1"/>
-    <col min="5" max="5" width="11.83203125" style="28" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.08203125" style="28" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" style="28" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" style="28" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" style="28" customWidth="1"/>
+    <col min="4" max="4" width="27.7109375" style="28" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="28" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="28" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9" style="28"/>
   </cols>
   <sheetData>
@@ -8481,25 +8490,278 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A6ACB90-8E38-47AA-9917-B39EDD39CA67}">
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2">
+        <v>10511434</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>10375000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>10488088</v>
+      </c>
+      <c r="C3">
+        <v>7159317</v>
+      </c>
+      <c r="D3">
+        <v>6516500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>10442000</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>10442000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>9482232</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>9482232</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>10988489</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12">
+        <v>9381404</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>8902000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>11488776</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>11339657</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15">
+        <v>7713158</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>7713158</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16">
+        <v>10719153</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>10719153</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17">
+        <v>18894208</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>9482232</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92EAFC54-4873-4634-A347-9827E9C5CD68}">
   <sheetPr>
     <tabColor rgb="FF002060"/>
   </sheetPr>
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.75" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.08203125" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="34">
+    <row r="1" spans="1:4" ht="30">
       <c r="A1" s="3" t="s">
         <v>21</v>
       </c>
@@ -8668,13 +8930,16 @@
         <v>14</v>
       </c>
       <c r="B12" s="2">
-        <v>0</v>
+        <f>'US values'!B12</f>
+        <v>9381404</v>
       </c>
       <c r="C12" s="2">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
+        <f>'US values'!C12</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="2">
+        <f>'US values'!D12</f>
+        <v>8902000</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -8712,13 +8977,16 @@
         <v>18</v>
       </c>
       <c r="B15" s="2">
-        <v>0</v>
+        <f>'US values'!B15</f>
+        <v>7713158</v>
       </c>
       <c r="C15" s="2">
+        <f>'US values'!C15</f>
         <v>0</v>
       </c>
       <c r="D15" s="2">
-        <v>0</v>
+        <f>'US values'!D15</f>
+        <v>7713158</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -8742,13 +9010,16 @@
         <v>20</v>
       </c>
       <c r="B17" s="2">
-        <v>0</v>
+        <f>'US values'!B17</f>
+        <v>18894208</v>
       </c>
       <c r="C17" s="2">
+        <f>'US values'!C17</f>
         <v>0</v>
       </c>
       <c r="D17" s="2">
-        <v>0</v>
+        <f>'US values'!D17</f>
+        <v>9482232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
NEXT Group edit to natural gas heat rate
</commit_message>
<xml_diff>
--- a/InputData/elec/BHRbEF/BAU Heat Rate by Electricity Fuel.xlsx
+++ b/InputData/elec/BHRbEF/BAU Heat Rate by Electricity Fuel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-southkorea\InputData\elec\BHRbEF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973C5770-C914-4F63-970F-96E30DA96C55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6EC72AF-D0C4-45BB-813F-DCCF61B5432A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,8 @@
     <sheet name="outlook of power" sheetId="20" r:id="rId5"/>
     <sheet name="Cal" sheetId="14" r:id="rId6"/>
     <sheet name="US values" sheetId="22" r:id="rId7"/>
-    <sheet name="BHRbEF" sheetId="17" r:id="rId8"/>
+    <sheet name="natural gas" sheetId="23" r:id="rId8"/>
+    <sheet name="BHRbEF" sheetId="17" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="217">
   <si>
     <t>BAU Heat Rate by Electricity Fuel</t>
   </si>
@@ -1021,6 +1022,21 @@
   </si>
   <si>
     <t>Where there is no Korea data available, we use US values from the US EPS.</t>
+  </si>
+  <si>
+    <t>Energy efficiency of CCGT:</t>
+  </si>
+  <si>
+    <t>Heat rate:</t>
+  </si>
+  <si>
+    <t>Generation:</t>
+  </si>
+  <si>
+    <t>MWh</t>
+  </si>
+  <si>
+    <t>BTU</t>
   </si>
 </sst>
 </file>
@@ -1457,7 +1473,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
@@ -1467,8 +1483,9 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1646,25 +1663,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1673,13 +1684,24 @@
     <xf numFmtId="0" fontId="13" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Note" xfId="4" builtinId="10"/>
+    <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2006,10 +2028,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V42"/>
+  <dimension ref="A1:V43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2359,31 +2381,46 @@
       <c r="U35"/>
       <c r="V35"/>
     </row>
-    <row r="36" spans="1:22">
+    <row r="36" spans="1:22" s="67" customFormat="1">
+      <c r="C36" s="33" t="s">
+        <v>215</v>
+      </c>
+      <c r="D36" s="67">
+        <f>3412000</f>
+        <v>3412000</v>
+      </c>
+      <c r="E36" s="67" t="s">
+        <v>216</v>
+      </c>
       <c r="T36"/>
       <c r="U36"/>
       <c r="V36"/>
     </row>
     <row r="37" spans="1:22">
-      <c r="B37" s="33" t="s">
+      <c r="T37"/>
+      <c r="U37"/>
+      <c r="V37"/>
+    </row>
+    <row r="38" spans="1:22">
+      <c r="B38" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="C37" s="4">
+      <c r="C38" s="4">
         <v>2019</v>
       </c>
     </row>
-    <row r="39" spans="1:22">
-      <c r="A39" s="62" t="s">
+    <row r="40" spans="1:22">
+      <c r="A40" s="62" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="40" spans="1:22">
-      <c r="A40" s="4" t="s">
+    <row r="41" spans="1:22">
+      <c r="A41" s="4" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="42" spans="1:22">
-      <c r="A42" s="4" t="s">
+    <row r="43" spans="1:22">
+      <c r="A43" s="4" t="s">
         <v>211</v>
       </c>
     </row>
@@ -2416,14 +2453,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="45" customHeight="1">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="68" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="4" t="s">
@@ -5365,35 +5402,35 @@
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="74" t="s">
         <v>108</v>
       </c>
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="74" t="s">
         <v>109</v>
       </c>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69" t="s">
+      <c r="C2" s="74"/>
+      <c r="D2" s="74" t="s">
         <v>110</v>
       </c>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69" t="s">
+      <c r="E2" s="74"/>
+      <c r="F2" s="74" t="s">
         <v>111</v>
       </c>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69" t="s">
+      <c r="G2" s="74"/>
+      <c r="H2" s="74" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="69"/>
-      <c r="J2" s="69" t="s">
+      <c r="I2" s="74"/>
+      <c r="J2" s="74" t="s">
         <v>31</v>
       </c>
-      <c r="K2" s="69"/>
-      <c r="L2" s="69" t="s">
+      <c r="K2" s="74"/>
+      <c r="L2" s="74" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A3" s="70"/>
+      <c r="A3" s="75"/>
       <c r="B3" s="37" t="s">
         <v>113</v>
       </c>
@@ -5424,7 +5461,7 @@
       <c r="K3" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="L3" s="70"/>
+      <c r="L3" s="75"/>
     </row>
     <row r="4" spans="1:12" ht="15.75" thickTop="1">
       <c r="A4" s="44">
@@ -5856,34 +5893,34 @@
       <c r="A17" s="71" t="s">
         <v>108</v>
       </c>
-      <c r="B17" s="69" t="s">
+      <c r="B17" s="74" t="s">
         <v>132</v>
       </c>
-      <c r="C17" s="69"/>
-      <c r="D17" s="69"/>
+      <c r="C17" s="74"/>
+      <c r="D17" s="74"/>
       <c r="E17" s="71"/>
-      <c r="F17" s="73" t="s">
+      <c r="F17" s="70" t="s">
         <v>116</v>
       </c>
-      <c r="G17" s="69"/>
-      <c r="H17" s="69"/>
-      <c r="I17" s="69"/>
+      <c r="G17" s="74"/>
+      <c r="H17" s="74"/>
+      <c r="I17" s="74"/>
       <c r="J17" s="71"/>
-      <c r="K17" s="73" t="s">
+      <c r="K17" s="70" t="s">
         <v>134</v>
       </c>
-      <c r="L17" s="69"/>
+      <c r="L17" s="74"/>
       <c r="M17" s="71"/>
-      <c r="N17" s="74" t="s">
+      <c r="N17" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="O17" s="74" t="s">
+      <c r="O17" s="72" t="s">
         <v>28</v>
       </c>
-      <c r="P17" s="74" t="s">
+      <c r="P17" s="72" t="s">
         <v>117</v>
       </c>
-      <c r="Q17" s="74" t="s">
+      <c r="Q17" s="72" t="s">
         <v>118</v>
       </c>
       <c r="R17" s="41" t="s">
@@ -5892,24 +5929,24 @@
       <c r="S17" s="41" t="s">
         <v>136</v>
       </c>
-      <c r="T17" s="74" t="s">
+      <c r="T17" s="72" t="s">
         <v>29</v>
       </c>
-      <c r="U17" s="74" t="s">
+      <c r="U17" s="72" t="s">
         <v>52</v>
       </c>
-      <c r="V17" s="73" t="s">
+      <c r="V17" s="70" t="s">
         <v>119</v>
       </c>
-      <c r="W17" s="69"/>
+      <c r="W17" s="74"/>
       <c r="X17" s="71"/>
-      <c r="Y17" s="73" t="s">
+      <c r="Y17" s="70" t="s">
         <v>120</v>
       </c>
       <c r="Z17" s="71"/>
     </row>
     <row r="18" spans="1:26" ht="27.75" thickBot="1">
-      <c r="A18" s="72"/>
+      <c r="A18" s="76"/>
       <c r="B18" s="37" t="s">
         <v>121</v>
       </c>
@@ -5946,18 +5983,18 @@
       <c r="M18" s="38" t="s">
         <v>125</v>
       </c>
-      <c r="N18" s="75"/>
-      <c r="O18" s="75"/>
-      <c r="P18" s="75"/>
-      <c r="Q18" s="75"/>
+      <c r="N18" s="73"/>
+      <c r="O18" s="73"/>
+      <c r="P18" s="73"/>
+      <c r="Q18" s="73"/>
       <c r="R18" s="40" t="s">
         <v>137</v>
       </c>
       <c r="S18" s="40" t="s">
         <v>137</v>
       </c>
-      <c r="T18" s="75"/>
-      <c r="U18" s="75"/>
+      <c r="T18" s="73"/>
+      <c r="U18" s="73"/>
       <c r="V18" s="39" t="s">
         <v>126</v>
       </c>
@@ -6881,14 +6918,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="Y17:Z17"/>
-    <mergeCell ref="N17:N18"/>
-    <mergeCell ref="O17:O18"/>
-    <mergeCell ref="P17:P18"/>
-    <mergeCell ref="Q17:Q18"/>
-    <mergeCell ref="T17:T18"/>
-    <mergeCell ref="U17:U18"/>
-    <mergeCell ref="V17:X17"/>
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="B17:E17"/>
@@ -6900,6 +6929,14 @@
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="J2:K2"/>
+    <mergeCell ref="Y17:Z17"/>
+    <mergeCell ref="N17:N18"/>
+    <mergeCell ref="O17:O18"/>
+    <mergeCell ref="P17:P18"/>
+    <mergeCell ref="Q17:Q18"/>
+    <mergeCell ref="T17:T18"/>
+    <mergeCell ref="U17:U18"/>
+    <mergeCell ref="V17:X17"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8141,7 +8178,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="35">
-        <f>INDEX(BFPaT_biomass!$B$103:$E$103,,MATCH(About!$C$37,BFPaT_biomass!$B$101:$E$101,0))</f>
+        <f>INDEX(BFPaT_biomass!$B$103:$E$103,,MATCH(About!$C$38,BFPaT_biomass!$B$101:$E$101,0))</f>
         <v>3002318.2</v>
       </c>
       <c r="C2" s="35">
@@ -8179,15 +8216,15 @@
         <v>17</v>
       </c>
       <c r="B4" s="35">
-        <f>INDEX('fuel consumption &amp; power'!$B$4:$B$14,MATCH(About!$C$37,'fuel consumption &amp; power'!$A$4:$A$14,0))*1000</f>
+        <f>INDEX('fuel consumption &amp; power'!$B$4:$B$14,MATCH(About!$C$38,'fuel consumption &amp; power'!$A$4:$A$14,0))*1000</f>
         <v>1164840</v>
       </c>
       <c r="C4" s="35">
-        <f>INDEX('fuel consumption &amp; power'!$C$4:$C$14,MATCH(About!$C$37,'fuel consumption &amp; power'!$A$4:$A$14,0))*About!$D$34*1000</f>
+        <f>INDEX('fuel consumption &amp; power'!$C$4:$C$14,MATCH(About!$C$38,'fuel consumption &amp; power'!$A$4:$A$14,0))*About!$D$34*1000</f>
         <v>20536563.142620001</v>
       </c>
       <c r="D4" s="35">
-        <f>INDEX('fuel consumption &amp; power'!$F$19:$F$29,MATCH(About!$C$37,'fuel consumption &amp; power'!$A$4:$A$14,0))</f>
+        <f>INDEX('fuel consumption &amp; power'!$F$19:$F$29,MATCH(About!$C$38,'fuel consumption &amp; power'!$A$4:$A$14,0))</f>
         <v>2559357</v>
       </c>
       <c r="E4" s="35">
@@ -8218,15 +8255,15 @@
         <v>5</v>
       </c>
       <c r="B6" s="35">
-        <f>INDEX('fuel consumption &amp; power'!$J$4:$J$14,MATCH(About!$C$37,'fuel consumption &amp; power'!$A$4:$A$14,0))*1000</f>
+        <f>INDEX('fuel consumption &amp; power'!$J$4:$J$14,MATCH(About!$C$38,'fuel consumption &amp; power'!$A$4:$A$14,0))*1000</f>
         <v>8890733</v>
       </c>
       <c r="C6" s="35">
-        <f>INDEX('fuel consumption &amp; power'!$K$4:$K$14,MATCH(About!$C$37,'fuel consumption &amp; power'!$A$4:$A$14,0))*About!$D$34*1000</f>
+        <f>INDEX('fuel consumption &amp; power'!$K$4:$K$14,MATCH(About!$C$38,'fuel consumption &amp; power'!$A$4:$A$14,0))*About!$D$34*1000</f>
         <v>51421530.253229998</v>
       </c>
       <c r="D6" s="35">
-        <f>INDEX('fuel consumption &amp; power'!$R$20:$R$29,MATCH(About!$C$37,'fuel consumption &amp; power'!$A$4:$A$14,0))</f>
+        <f>INDEX('fuel consumption &amp; power'!$R$20:$R$29,MATCH(About!$C$38,'fuel consumption &amp; power'!$A$4:$A$14,0))</f>
         <v>116512939</v>
       </c>
       <c r="E6" s="35">
@@ -8257,7 +8294,7 @@
         <v>0</v>
       </c>
       <c r="D8" s="35">
-        <f>INDEX('fuel consumption &amp; power'!$N$19:$N$29,MATCH(About!$C$37,'fuel consumption &amp; power'!$A$4:$A$14,0))</f>
+        <f>INDEX('fuel consumption &amp; power'!$N$19:$N$29,MATCH(About!$C$38,'fuel consumption &amp; power'!$A$4:$A$14,0))</f>
         <v>145909669.5</v>
       </c>
       <c r="E8" s="35">
@@ -8287,15 +8324,15 @@
         <v>13</v>
       </c>
       <c r="B10" s="35">
-        <f>INDEX('fuel consumption &amp; power'!$H$4:$H$14,MATCH(About!$C$37,'fuel consumption &amp; power'!$A$4:$A$14,0))*1000</f>
+        <f>INDEX('fuel consumption &amp; power'!$H$4:$H$14,MATCH(About!$C$38,'fuel consumption &amp; power'!$A$4:$A$14,0))*1000</f>
         <v>322568</v>
       </c>
       <c r="C10" s="35">
-        <f>INDEX('fuel consumption &amp; power'!$I$4:$I$14,MATCH(About!$C$37,'fuel consumption &amp; power'!$A$4:$A$14,0))*About!$D$34*1000</f>
+        <f>INDEX('fuel consumption &amp; power'!$I$4:$I$14,MATCH(About!$C$38,'fuel consumption &amp; power'!$A$4:$A$14,0))*About!$D$34*1000</f>
         <v>35387795.043449998</v>
       </c>
       <c r="D10" s="35">
-        <f>INDEX('fuel consumption &amp; power'!$S$19:$S$29,MATCH(About!$C$37,'fuel consumption &amp; power'!$A$4:$A$14,0))</f>
+        <f>INDEX('fuel consumption &amp; power'!$S$19:$S$29,MATCH(About!$C$38,'fuel consumption &amp; power'!$A$4:$A$14,0))</f>
         <v>2006685</v>
       </c>
       <c r="E10" s="35">
@@ -8383,15 +8420,15 @@
         <v>15</v>
       </c>
       <c r="B15" s="35">
-        <f>INDEX('fuel consumption &amp; power'!$D$4:$D$14,MATCH(About!$C$37,'fuel consumption &amp; power'!$A$4:$A$14,0))*1000</f>
+        <f>INDEX('fuel consumption &amp; power'!$D$4:$D$14,MATCH(About!$C$38,'fuel consumption &amp; power'!$A$4:$A$14,0))*1000</f>
         <v>83321351</v>
       </c>
       <c r="C15" s="35">
-        <f>INDEX('fuel consumption &amp; power'!$E$4:$E$14,MATCH(About!$C$37,'fuel consumption &amp; power'!$A$4:$A$14,0))*About!$D$34*1000</f>
+        <f>INDEX('fuel consumption &amp; power'!$E$4:$E$14,MATCH(About!$C$38,'fuel consumption &amp; power'!$A$4:$A$14,0))*About!$D$34*1000</f>
         <v>21830819.032169998</v>
       </c>
       <c r="D15" s="35">
-        <f>INDEX('fuel consumption &amp; power'!$G$19:$G$29,MATCH(About!$C$37,'fuel consumption &amp; power'!$A$4:$A$14,0))</f>
+        <f>INDEX('fuel consumption &amp; power'!$G$19:$G$29,MATCH(About!$C$38,'fuel consumption &amp; power'!$A$4:$A$14,0))</f>
         <v>214478728</v>
       </c>
       <c r="E15" s="35">
@@ -8404,15 +8441,15 @@
         <v>19</v>
       </c>
       <c r="B16" s="35">
-        <f>INDEX('fuel consumption &amp; power'!$F$4:$F$14,MATCH(About!$C$37,'fuel consumption &amp; power'!$A$4:$A$14,0))*1000</f>
+        <f>INDEX('fuel consumption &amp; power'!$F$4:$F$14,MATCH(About!$C$38,'fuel consumption &amp; power'!$A$4:$A$14,0))*1000</f>
         <v>361925</v>
       </c>
       <c r="C16" s="35">
-        <f>INDEX('fuel consumption &amp; power'!$G$4:$G$14,MATCH(About!$C$37,'fuel consumption &amp; power'!$A$4:$A$14,0))*About!$D$34*1000</f>
+        <f>INDEX('fuel consumption &amp; power'!$G$4:$G$14,MATCH(About!$C$38,'fuel consumption &amp; power'!$A$4:$A$14,0))*About!$D$34*1000</f>
         <v>39498410.281949997</v>
       </c>
       <c r="D16" s="35">
-        <f>INDEX('fuel consumption &amp; power'!$H$19:$H$29,MATCH(About!$C$37,'fuel consumption &amp; power'!$A$4:$A$14,0))</f>
+        <f>INDEX('fuel consumption &amp; power'!$H$19:$H$29,MATCH(About!$C$38,'fuel consumption &amp; power'!$A$4:$A$14,0))</f>
         <v>1285568</v>
       </c>
       <c r="E16" s="35">
@@ -8448,7 +8485,7 @@
         <v>198</v>
       </c>
       <c r="B21" s="28">
-        <f>INDEX('heat of nuclear gen'!$C$23:$L$23,,MATCH(About!$C$37,'heat of nuclear gen'!$C$2:$L$2,0))</f>
+        <f>INDEX('heat of nuclear gen'!$C$23:$L$23,,MATCH(About!$C$38,'heat of nuclear gen'!$C$2:$L$2,0))</f>
         <v>31079</v>
       </c>
       <c r="C21" s="28" t="s">
@@ -8743,20 +8780,69 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB53C90A-75AF-4582-B40E-8DE849FD153E}">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="77">
+        <v>0.46949999999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5">
+        <v>109397542</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8">
+        <f>A5/A2*About!D36/A5</f>
+        <v>7267305.6443024492</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92EAFC54-4873-4634-A347-9827E9C5CD68}">
   <sheetPr>
     <tabColor rgb="FF002060"/>
   </sheetPr>
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.140625" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
   </cols>
@@ -8796,15 +8882,15 @@
         <v>5</v>
       </c>
       <c r="B3" s="2">
-        <f>Cal!E6</f>
-        <v>3923813.95454191</v>
+        <f>'natural gas'!A8</f>
+        <v>7267305.6443024492</v>
       </c>
       <c r="C3" s="2">
         <v>0</v>
       </c>
       <c r="D3" s="2">
-        <f>B3*'outlook of power'!D6</f>
-        <v>3571283.7945635351</v>
+        <f>'natural gas'!A8</f>
+        <v>7267305.6443024492</v>
       </c>
     </row>
     <row r="4" spans="1:4">

</xml_diff>

<commit_message>
Update heat rates for new plants with IEA data
</commit_message>
<xml_diff>
--- a/InputData/elec/BHRbEF/BAU Heat Rate by Electricity Fuel.xlsx
+++ b/InputData/elec/BHRbEF/BAU Heat Rate by Electricity Fuel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-southkorea\InputData\elec\BHRbEF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6EC72AF-D0C4-45BB-813F-DCCF61B5432A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0716DE96-9D76-4DA6-B054-567585710A31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,10 +20,14 @@
     <sheet name="outlook of power" sheetId="20" r:id="rId5"/>
     <sheet name="Cal" sheetId="14" r:id="rId6"/>
     <sheet name="US values" sheetId="22" r:id="rId7"/>
-    <sheet name="natural gas" sheetId="23" r:id="rId8"/>
-    <sheet name="BHRbEF" sheetId="17" r:id="rId9"/>
+    <sheet name="existing natural gas" sheetId="24" r:id="rId8"/>
+    <sheet name="IEA heat rates" sheetId="23" r:id="rId9"/>
+    <sheet name="BHRbEF" sheetId="17" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <externalReferences>
+    <externalReference r:id="rId11"/>
+  </externalReferences>
+  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="221">
   <si>
     <t>BAU Heat Rate by Electricity Fuel</t>
   </si>
@@ -847,14 +851,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>KESIS</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://www.kesis.net/sub/subChart.jsp?report_id=920308&amp;reportType=0</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>항목1*</t>
   </si>
   <si>
@@ -997,22 +993,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>Heat rate (nuclear power)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Primary energy output of nuclear power</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Annual primary energy supply</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Newly built assumption</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>MOTIE</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -1037,16 +1017,48 @@
   </si>
   <si>
     <t>BTU</t>
+  </si>
+  <si>
+    <t>btu/kWh</t>
+  </si>
+  <si>
+    <t>efficiency</t>
+  </si>
+  <si>
+    <t>heat rate in btu/kWh</t>
+  </si>
+  <si>
+    <t>btu/MWh</t>
+  </si>
+  <si>
+    <t>Newly built assumption, other plant types</t>
+  </si>
+  <si>
+    <t>Newly built assumption, coal, natural gas nonpeaker, nuclear</t>
+  </si>
+  <si>
+    <t>IEA</t>
+  </si>
+  <si>
+    <t>Projected Costs of Generating Electricity</t>
+  </si>
+  <si>
+    <t>https://iea.blob.core.windows.net/assets/ae17da3d-e8a5-4163-a3ec-2e6fb0b5677d/Projected-Costs-of-Generating-Electricity-2020.pdf</t>
+  </si>
+  <si>
+    <t>Tables 3.11 - 3.13</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="5">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="#,##0.0#"/>
+    <numFmt numFmtId="168" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -1473,7 +1485,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
@@ -1484,8 +1496,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1666,16 +1679,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1684,18 +1710,10 @@
     <xf numFmtId="0" fontId="13" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
+    <cellStyle name="Comma" xfId="6" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1763,6 +1781,178 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>46778</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>142463</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{431908BE-1E6D-4E22-AABF-57EC5C3D5309}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="257175" y="1609725"/>
+          <a:ext cx="6771428" cy="3295238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>227719</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>75882</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D276F72E-1981-48AC-910D-5F54DC4AE91D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="161925" y="4581525"/>
+          <a:ext cx="7047619" cy="2542857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>180101</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>180714</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E985317-C0C0-43FE-818C-7F5940617EB9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="171450" y="8572500"/>
+          <a:ext cx="6990476" cy="2085714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="About"/>
+      <sheetName val="BFPaT_biomass"/>
+      <sheetName val="fuel consumption &amp; power"/>
+      <sheetName val="heat of nuclear gen"/>
+      <sheetName val="outlook of power"/>
+      <sheetName val="Cal"/>
+      <sheetName val="US values"/>
+      <sheetName val="natural gas"/>
+      <sheetName val="BHRbEF"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="36">
+          <cell r="D36">
+            <v>3412000</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2030,8 +2220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2053,7 +2243,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="60" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="R3"/>
       <c r="S3"/>
@@ -2092,7 +2282,7 @@
     </row>
     <row r="6" spans="1:19">
       <c r="B6" s="31" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="H6"/>
       <c r="I6"/>
@@ -2171,7 +2361,7 @@
     </row>
     <row r="11" spans="1:19">
       <c r="B11" s="31" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="G11" s="64"/>
       <c r="H11" s="64"/>
@@ -2231,7 +2421,7 @@
     </row>
     <row r="16" spans="1:19">
       <c r="B16" s="31" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="17" spans="1:22">
@@ -2247,48 +2437,61 @@
     <row r="19" spans="1:22">
       <c r="B19" s="31"/>
     </row>
-    <row r="20" spans="1:22">
+    <row r="20" spans="1:22" s="68" customFormat="1">
+      <c r="A20" s="32"/>
       <c r="B20" s="61" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="21" spans="1:22">
+        <v>216</v>
+      </c>
+      <c r="T20"/>
+      <c r="U20"/>
+      <c r="V20"/>
+    </row>
+    <row r="21" spans="1:22" s="68" customFormat="1">
+      <c r="A21" s="32"/>
       <c r="B21" s="31" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="22" spans="1:22">
+        <v>217</v>
+      </c>
+      <c r="T21"/>
+      <c r="U21"/>
+      <c r="V21"/>
+    </row>
+    <row r="22" spans="1:22" s="68" customFormat="1">
+      <c r="A22" s="32"/>
       <c r="B22" s="31">
         <v>2020</v>
       </c>
-    </row>
-    <row r="23" spans="1:22">
+      <c r="T22"/>
+      <c r="U22"/>
+      <c r="V22"/>
+    </row>
+    <row r="23" spans="1:22" s="68" customFormat="1">
+      <c r="A23" s="32"/>
       <c r="B23" s="31" t="s">
-        <v>206</v>
+        <v>218</v>
       </c>
       <c r="T23"/>
       <c r="U23"/>
       <c r="V23"/>
     </row>
-    <row r="24" spans="1:22">
-      <c r="A24" s="30"/>
+    <row r="24" spans="1:22" s="68" customFormat="1">
+      <c r="A24" s="32"/>
       <c r="B24" s="55" t="s">
-        <v>163</v>
+        <v>219</v>
       </c>
       <c r="T24"/>
       <c r="U24"/>
       <c r="V24"/>
     </row>
-    <row r="25" spans="1:22">
+    <row r="25" spans="1:22" s="68" customFormat="1">
       <c r="A25" s="32"/>
       <c r="B25" s="31" t="s">
-        <v>207</v>
+        <v>220</v>
       </c>
       <c r="T25"/>
       <c r="U25"/>
       <c r="V25"/>
     </row>
-    <row r="26" spans="1:22">
+    <row r="26" spans="1:22" s="68" customFormat="1">
       <c r="A26" s="32"/>
       <c r="B26" s="31"/>
       <c r="T26"/>
@@ -2298,7 +2501,7 @@
     <row r="27" spans="1:22">
       <c r="A27" s="32"/>
       <c r="B27" s="61" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="T27"/>
       <c r="U27"/>
@@ -2306,7 +2509,7 @@
     </row>
     <row r="28" spans="1:22">
       <c r="B28" s="31" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="T28"/>
       <c r="U28"/>
@@ -2322,7 +2525,7 @@
     </row>
     <row r="30" spans="1:22">
       <c r="B30" s="31" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="T30"/>
       <c r="U30"/>
@@ -2383,14 +2586,14 @@
     </row>
     <row r="36" spans="1:22" s="67" customFormat="1">
       <c r="C36" s="33" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="D36" s="67">
         <f>3412000</f>
         <v>3412000</v>
       </c>
       <c r="E36" s="67" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="T36"/>
       <c r="U36"/>
@@ -2411,17 +2614,17 @@
     </row>
     <row r="40" spans="1:22">
       <c r="A40" s="62" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="41" spans="1:22">
       <c r="A41" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="43" spans="1:22">
       <c r="A43" s="4" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -2431,10 +2634,296 @@
     <hyperlink ref="B12" r:id="rId2" xr:uid="{CD43BEE1-2D97-4F10-8516-E6F4D1F17381}"/>
     <hyperlink ref="B17" r:id="rId3" xr:uid="{E9ADE772-A738-491D-BFD2-CB6B0D9F34D8}"/>
     <hyperlink ref="B31" r:id="rId4" xr:uid="{CA3FAF32-8045-4909-9A8D-889D0D972CFA}"/>
-    <hyperlink ref="B24" r:id="rId5" xr:uid="{2161AA0F-4ABE-4768-BE4A-937F4630E508}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92EAFC54-4873-4634-A347-9827E9C5CD68}">
+  <sheetPr>
+    <tabColor rgb="FF002060"/>
+  </sheetPr>
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="30">
+      <c r="A1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="2">
+        <f>Cal!E4</f>
+        <v>9346804.7681700829</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2">
+        <f>'IEA heat rates'!A43</f>
+        <v>7934883.7209302327</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2">
+        <f>'existing natural gas'!A8</f>
+        <v>7267305.6443024492</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
+        <f>'IEA heat rates'!A23</f>
+        <v>5933913.0434782607</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2">
+        <f>'IEA heat rates'!A61</f>
+        <v>9477777.777777778</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
+        <f>'IEA heat rates'!A61</f>
+        <v>9477777.777777778</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="2">
+        <f>Cal!E2</f>
+        <v>10011408.509574568</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2">
+        <f>B9</f>
+        <v>10011408.509574568</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="2">
+        <f>Cal!E10</f>
+        <v>5688471.4200662179</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2">
+        <f>B11</f>
+        <v>5688471.4200662179</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="2">
+        <f>'US values'!B12</f>
+        <v>9381404</v>
+      </c>
+      <c r="C12" s="2">
+        <f>'US values'!C12</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="2">
+        <f>'US values'!D12</f>
+        <v>8902000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="2">
+        <f>Cal!E15</f>
+        <v>8480903.2213064823</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2">
+        <f>B13*'outlook of power'!C6</f>
+        <v>6276708.0771550443</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="2">
+        <f>'US values'!B15</f>
+        <v>7713158</v>
+      </c>
+      <c r="C15" s="2">
+        <f>'US values'!C15</f>
+        <v>0</v>
+      </c>
+      <c r="D15" s="2">
+        <f>'US values'!D15</f>
+        <v>7713158</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="2">
+        <f>Cal!E16</f>
+        <v>11119957.980670609</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2">
+        <f>B16</f>
+        <v>11119957.980670609</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="2">
+        <f>'US values'!B17</f>
+        <v>18894208</v>
+      </c>
+      <c r="C17" s="2">
+        <f>'US values'!C17</f>
+        <v>0</v>
+      </c>
+      <c r="D17" s="2">
+        <f>'US values'!D17</f>
+        <v>9482232</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2453,14 +2942,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="45" customHeight="1">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="70" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="4" t="s">
@@ -5402,35 +5891,35 @@
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="74" t="s">
+      <c r="A2" s="72" t="s">
         <v>108</v>
       </c>
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="72" t="s">
         <v>109</v>
       </c>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74" t="s">
+      <c r="C2" s="72"/>
+      <c r="D2" s="72" t="s">
         <v>110</v>
       </c>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74" t="s">
+      <c r="E2" s="72"/>
+      <c r="F2" s="72" t="s">
         <v>111</v>
       </c>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74" t="s">
+      <c r="G2" s="72"/>
+      <c r="H2" s="72" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="74"/>
-      <c r="J2" s="74" t="s">
+      <c r="I2" s="72"/>
+      <c r="J2" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="K2" s="74"/>
-      <c r="L2" s="74" t="s">
+      <c r="K2" s="72"/>
+      <c r="L2" s="72" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A3" s="75"/>
+      <c r="A3" s="73"/>
       <c r="B3" s="37" t="s">
         <v>113</v>
       </c>
@@ -5461,7 +5950,7 @@
       <c r="K3" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="L3" s="75"/>
+      <c r="L3" s="73"/>
     </row>
     <row r="4" spans="1:12" ht="15.75" thickTop="1">
       <c r="A4" s="44">
@@ -5890,37 +6379,37 @@
       </c>
     </row>
     <row r="17" spans="1:26">
-      <c r="A17" s="71" t="s">
+      <c r="A17" s="74" t="s">
         <v>108</v>
       </c>
-      <c r="B17" s="74" t="s">
+      <c r="B17" s="72" t="s">
         <v>132</v>
       </c>
-      <c r="C17" s="74"/>
-      <c r="D17" s="74"/>
-      <c r="E17" s="71"/>
-      <c r="F17" s="70" t="s">
+      <c r="C17" s="72"/>
+      <c r="D17" s="72"/>
+      <c r="E17" s="74"/>
+      <c r="F17" s="76" t="s">
         <v>116</v>
       </c>
-      <c r="G17" s="74"/>
-      <c r="H17" s="74"/>
-      <c r="I17" s="74"/>
-      <c r="J17" s="71"/>
-      <c r="K17" s="70" t="s">
+      <c r="G17" s="72"/>
+      <c r="H17" s="72"/>
+      <c r="I17" s="72"/>
+      <c r="J17" s="74"/>
+      <c r="K17" s="76" t="s">
         <v>134</v>
       </c>
-      <c r="L17" s="74"/>
-      <c r="M17" s="71"/>
-      <c r="N17" s="72" t="s">
+      <c r="L17" s="72"/>
+      <c r="M17" s="74"/>
+      <c r="N17" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="O17" s="72" t="s">
+      <c r="O17" s="77" t="s">
         <v>28</v>
       </c>
-      <c r="P17" s="72" t="s">
+      <c r="P17" s="77" t="s">
         <v>117</v>
       </c>
-      <c r="Q17" s="72" t="s">
+      <c r="Q17" s="77" t="s">
         <v>118</v>
       </c>
       <c r="R17" s="41" t="s">
@@ -5929,24 +6418,24 @@
       <c r="S17" s="41" t="s">
         <v>136</v>
       </c>
-      <c r="T17" s="72" t="s">
+      <c r="T17" s="77" t="s">
         <v>29</v>
       </c>
-      <c r="U17" s="72" t="s">
+      <c r="U17" s="77" t="s">
         <v>52</v>
       </c>
-      <c r="V17" s="70" t="s">
+      <c r="V17" s="76" t="s">
         <v>119</v>
       </c>
-      <c r="W17" s="74"/>
-      <c r="X17" s="71"/>
-      <c r="Y17" s="70" t="s">
+      <c r="W17" s="72"/>
+      <c r="X17" s="74"/>
+      <c r="Y17" s="76" t="s">
         <v>120</v>
       </c>
-      <c r="Z17" s="71"/>
+      <c r="Z17" s="74"/>
     </row>
     <row r="18" spans="1:26" ht="27.75" thickBot="1">
-      <c r="A18" s="76"/>
+      <c r="A18" s="75"/>
       <c r="B18" s="37" t="s">
         <v>121</v>
       </c>
@@ -5983,18 +6472,18 @@
       <c r="M18" s="38" t="s">
         <v>125</v>
       </c>
-      <c r="N18" s="73"/>
-      <c r="O18" s="73"/>
-      <c r="P18" s="73"/>
-      <c r="Q18" s="73"/>
+      <c r="N18" s="78"/>
+      <c r="O18" s="78"/>
+      <c r="P18" s="78"/>
+      <c r="Q18" s="78"/>
       <c r="R18" s="40" t="s">
         <v>137</v>
       </c>
       <c r="S18" s="40" t="s">
         <v>137</v>
       </c>
-      <c r="T18" s="73"/>
-      <c r="U18" s="73"/>
+      <c r="T18" s="78"/>
+      <c r="U18" s="78"/>
       <c r="V18" s="39" t="s">
         <v>126</v>
       </c>
@@ -6873,51 +7362,59 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="49" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="43" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B36" s="43" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="43" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B37" s="43" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="43" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B38" s="43" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="43" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B39" s="43" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="43" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B40" s="43" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="Y17:Z17"/>
+    <mergeCell ref="N17:N18"/>
+    <mergeCell ref="O17:O18"/>
+    <mergeCell ref="P17:P18"/>
+    <mergeCell ref="Q17:Q18"/>
+    <mergeCell ref="T17:T18"/>
+    <mergeCell ref="U17:U18"/>
+    <mergeCell ref="V17:X17"/>
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="B17:E17"/>
@@ -6929,14 +7426,6 @@
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="J2:K2"/>
-    <mergeCell ref="Y17:Z17"/>
-    <mergeCell ref="N17:N18"/>
-    <mergeCell ref="O17:O18"/>
-    <mergeCell ref="P17:P18"/>
-    <mergeCell ref="Q17:Q18"/>
-    <mergeCell ref="T17:T18"/>
-    <mergeCell ref="U17:U18"/>
-    <mergeCell ref="V17:X17"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6955,10 +7444,10 @@
   <sheetData>
     <row r="2" spans="1:12" s="52" customFormat="1" ht="26.1" customHeight="1">
       <c r="A2" s="56" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B2" s="56" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C2" s="59">
         <v>2010</v>
@@ -6993,10 +7482,10 @@
     </row>
     <row r="3" spans="1:12" s="52" customFormat="1" ht="27" hidden="1" customHeight="1">
       <c r="A3" s="57" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B3" s="57" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C3" s="58">
         <v>264053</v>
@@ -7031,10 +7520,10 @@
     </row>
     <row r="4" spans="1:12" s="52" customFormat="1" ht="27" hidden="1" customHeight="1">
       <c r="A4" s="57" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B4" s="57" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C4" s="58">
         <v>8.4</v>
@@ -7069,10 +7558,10 @@
     </row>
     <row r="5" spans="1:12" s="52" customFormat="1" ht="27" hidden="1" customHeight="1">
       <c r="A5" s="57" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B5" s="57" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C5" s="58">
         <v>77142</v>
@@ -7107,10 +7596,10 @@
     </row>
     <row r="6" spans="1:12" s="52" customFormat="1" ht="27" hidden="1" customHeight="1">
       <c r="A6" s="57" t="s">
+        <v>165</v>
+      </c>
+      <c r="B6" s="57" t="s">
         <v>167</v>
-      </c>
-      <c r="B6" s="57" t="s">
-        <v>169</v>
       </c>
       <c r="C6" s="58">
         <v>29.2</v>
@@ -7145,10 +7634,10 @@
     </row>
     <row r="7" spans="1:12" s="52" customFormat="1" ht="27" hidden="1" customHeight="1">
       <c r="A7" s="57" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B7" s="57" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C7" s="58">
         <v>6044</v>
@@ -7183,10 +7672,10 @@
     </row>
     <row r="8" spans="1:12" s="52" customFormat="1" ht="27" hidden="1" customHeight="1">
       <c r="A8" s="57" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B8" s="57" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C8" s="58">
         <v>2.2999999999999998</v>
@@ -7221,10 +7710,10 @@
     </row>
     <row r="9" spans="1:12" s="52" customFormat="1" ht="27" hidden="1" customHeight="1">
       <c r="A9" s="57" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B9" s="57" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C9" s="58">
         <v>71097</v>
@@ -7259,10 +7748,10 @@
     </row>
     <row r="10" spans="1:12" s="52" customFormat="1" ht="27" hidden="1" customHeight="1">
       <c r="A10" s="57" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B10" s="57" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C10" s="58">
         <v>26.9</v>
@@ -7297,10 +7786,10 @@
     </row>
     <row r="11" spans="1:12" s="52" customFormat="1" ht="27" hidden="1" customHeight="1">
       <c r="A11" s="57" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B11" s="57" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C11" s="58">
         <v>104500</v>
@@ -7335,10 +7824,10 @@
     </row>
     <row r="12" spans="1:12" s="52" customFormat="1" ht="27" hidden="1" customHeight="1">
       <c r="A12" s="57" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B12" s="57" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C12" s="58">
         <v>39.6</v>
@@ -7373,10 +7862,10 @@
     </row>
     <row r="13" spans="1:12" s="52" customFormat="1" ht="27" hidden="1" customHeight="1">
       <c r="A13" s="57" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B13" s="57" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C13" s="58">
         <v>46385</v>
@@ -7411,10 +7900,10 @@
     </row>
     <row r="14" spans="1:12" s="52" customFormat="1" ht="27" hidden="1" customHeight="1">
       <c r="A14" s="57" t="s">
+        <v>172</v>
+      </c>
+      <c r="B14" s="57" t="s">
         <v>174</v>
-      </c>
-      <c r="B14" s="57" t="s">
-        <v>176</v>
       </c>
       <c r="C14" s="58">
         <v>17.600000000000001</v>
@@ -7449,10 +7938,10 @@
     </row>
     <row r="15" spans="1:12" s="52" customFormat="1" ht="27" hidden="1" customHeight="1">
       <c r="A15" s="57" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B15" s="57" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C15" s="58">
         <v>10925</v>
@@ -7487,10 +7976,10 @@
     </row>
     <row r="16" spans="1:12" s="52" customFormat="1" ht="27" hidden="1" customHeight="1">
       <c r="A16" s="57" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B16" s="57" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C16" s="58">
         <v>4.0999999999999996</v>
@@ -7525,10 +8014,10 @@
     </row>
     <row r="17" spans="1:12" s="52" customFormat="1" ht="27" hidden="1" customHeight="1">
       <c r="A17" s="57" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B17" s="57" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C17" s="58">
         <v>47190</v>
@@ -7563,10 +8052,10 @@
     </row>
     <row r="18" spans="1:12" s="52" customFormat="1" ht="27" hidden="1" customHeight="1">
       <c r="A18" s="57" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B18" s="57" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C18" s="58">
         <v>17.899999999999999</v>
@@ -7601,10 +8090,10 @@
     </row>
     <row r="19" spans="1:12" s="52" customFormat="1" ht="27" hidden="1" customHeight="1">
       <c r="A19" s="57" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B19" s="57" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C19" s="58">
         <v>43008</v>
@@ -7639,10 +8128,10 @@
     </row>
     <row r="20" spans="1:12" s="52" customFormat="1" ht="27" hidden="1" customHeight="1">
       <c r="A20" s="57" t="s">
+        <v>179</v>
+      </c>
+      <c r="B20" s="57" t="s">
         <v>181</v>
-      </c>
-      <c r="B20" s="57" t="s">
-        <v>183</v>
       </c>
       <c r="C20" s="58">
         <v>16.3</v>
@@ -7677,10 +8166,10 @@
     </row>
     <row r="21" spans="1:12" s="52" customFormat="1" ht="27" hidden="1" customHeight="1">
       <c r="A21" s="57" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B21" s="57" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C21" s="58">
         <v>1392</v>
@@ -7715,10 +8204,10 @@
     </row>
     <row r="22" spans="1:12" s="52" customFormat="1" ht="27" hidden="1" customHeight="1">
       <c r="A22" s="57" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B22" s="57" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C22" s="58">
         <v>0.5</v>
@@ -7756,7 +8245,7 @@
         <v>26</v>
       </c>
       <c r="B23" s="57" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C23" s="58">
         <v>31948</v>
@@ -7794,7 +8283,7 @@
         <v>26</v>
       </c>
       <c r="B24" s="57" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C24" s="58">
         <v>12.1</v>
@@ -7829,10 +8318,10 @@
     </row>
     <row r="25" spans="1:12" s="52" customFormat="1" ht="27" hidden="1" customHeight="1">
       <c r="A25" s="57" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B25" s="57" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C25" s="58">
         <v>6064</v>
@@ -7867,10 +8356,10 @@
     </row>
     <row r="26" spans="1:12" s="52" customFormat="1" ht="27" hidden="1" customHeight="1">
       <c r="A26" s="57" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B26" s="57" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C26" s="58">
         <v>2.2999999999999998</v>
@@ -8482,7 +8971,7 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="28" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B21" s="28">
         <f>INDEX('heat of nuclear gen'!$C$23:$L$23,,MATCH(About!$C$38,'heat of nuclear gen'!$C$2:$L$2,0))</f>
@@ -8513,7 +9002,7 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="28" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -8780,31 +9269,28 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB53C90A-75AF-4582-B40E-8DE849FD153E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00702EB5-17BE-4182-B574-F39263252FE2}">
   <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="77">
+      <c r="A2" s="69">
         <v>0.46949999999999997</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5" spans="1:1">
@@ -8814,12 +9300,12 @@
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8">
-        <f>A5/A2*About!D36/A5</f>
+        <f>A5/A2*[1]About!D36/A5</f>
         <v>7267305.6443024492</v>
       </c>
     </row>
@@ -8829,288 +9315,123 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92EAFC54-4873-4634-A347-9827E9C5CD68}">
-  <sheetPr>
-    <tabColor rgb="FF002060"/>
-  </sheetPr>
-  <dimension ref="A1:D17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB53C90A-75AF-4582-B40E-8DE849FD153E}">
+  <dimension ref="A20:B61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30">
-      <c r="A1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="2">
-        <f>Cal!E4</f>
-        <v>9346804.7681700829</v>
-      </c>
-      <c r="C2" s="2">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2">
-        <f>B2*'outlook of power'!C6</f>
-        <v>6917560.9546605302</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="2">
-        <f>'natural gas'!A8</f>
-        <v>7267305.6443024492</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2">
-        <f>'natural gas'!A8</f>
-        <v>7267305.6443024492</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2">
-        <f>Cal!E8</f>
-        <v>8446942.4372179806</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0</v>
-      </c>
-      <c r="D4" s="2">
-        <f>B4*'outlook of power'!B6</f>
-        <v>8153419.3409439968</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="2">
-        <v>0</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="2">
-        <v>0</v>
-      </c>
-      <c r="C6" s="2">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="2">
-        <v>0</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="2">
-        <v>0</v>
-      </c>
-      <c r="C8" s="2">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="2">
-        <f>Cal!E2</f>
-        <v>10011408.509574568</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0</v>
-      </c>
-      <c r="D9" s="2">
-        <f>B9</f>
-        <v>10011408.509574568</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="2">
-        <v>0</v>
-      </c>
-      <c r="C10" s="2">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="2">
-        <f>Cal!E10</f>
-        <v>5688471.4200662179</v>
-      </c>
-      <c r="C11" s="2">
-        <v>0</v>
-      </c>
-      <c r="D11" s="2">
-        <f>B11</f>
-        <v>5688471.4200662179</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="2">
-        <f>'US values'!B12</f>
-        <v>9381404</v>
-      </c>
-      <c r="C12" s="2">
-        <f>'US values'!C12</f>
-        <v>0</v>
-      </c>
-      <c r="D12" s="2">
-        <f>'US values'!D12</f>
-        <v>8902000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="2">
-        <f>Cal!E15</f>
-        <v>8480903.2213064823</v>
-      </c>
-      <c r="C13" s="2">
-        <v>0</v>
-      </c>
-      <c r="D13" s="2">
-        <f>B13*'outlook of power'!C6</f>
-        <v>6276708.0771550443</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="2">
-        <v>0</v>
-      </c>
-      <c r="C14" s="2">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="2">
-        <f>'US values'!B15</f>
-        <v>7713158</v>
-      </c>
-      <c r="C15" s="2">
-        <f>'US values'!C15</f>
-        <v>0</v>
-      </c>
-      <c r="D15" s="2">
-        <f>'US values'!D15</f>
-        <v>7713158</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="2">
-        <f>Cal!E16</f>
-        <v>11119957.980670609</v>
-      </c>
-      <c r="C16" s="2">
-        <v>0</v>
-      </c>
-      <c r="D16" s="2">
-        <f>B16</f>
-        <v>11119957.980670609</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="2">
-        <f>'US values'!B17</f>
-        <v>18894208</v>
-      </c>
-      <c r="C17" s="2">
-        <f>'US values'!C17</f>
-        <v>0</v>
-      </c>
-      <c r="D17" s="2">
-        <f>'US values'!D17</f>
-        <v>9482232</v>
+    <row r="20" spans="1:2">
+      <c r="A20">
+        <v>3412</v>
+      </c>
+      <c r="B20" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21">
+        <f>AVERAGE(0.56,0.59)</f>
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="B21" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22">
+        <f>A20/A21</f>
+        <v>5933.913043478261</v>
+      </c>
+      <c r="B22" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="79">
+        <f>A22*1000</f>
+        <v>5933913.0434782607</v>
+      </c>
+      <c r="B23" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40">
+        <v>3412</v>
+      </c>
+      <c r="B40" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41">
+        <v>0.43</v>
+      </c>
+      <c r="B41" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42">
+        <f>A40/A41</f>
+        <v>7934.8837209302328</v>
+      </c>
+      <c r="B42" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="79">
+        <f>A42*1000</f>
+        <v>7934883.7209302327</v>
+      </c>
+      <c r="B43" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58">
+        <v>3412</v>
+      </c>
+      <c r="B58" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59">
+        <v>0.36</v>
+      </c>
+      <c r="B59" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60">
+        <f>A58/A59</f>
+        <v>9477.7777777777774</v>
+      </c>
+      <c r="B60" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="79">
+        <f>A60*1000</f>
+        <v>9477777.777777778</v>
+      </c>
+      <c r="B61" t="s">
+        <v>214</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>